<commit_message>
Erste Version Dashboard erstellt
</commit_message>
<xml_diff>
--- a/Spitalliste_bereinigt_fuer_Dashboard.xlsx
+++ b/Spitalliste_bereinigt_fuer_Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina Frei\Documents\Studium\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56F2DB7-A9CD-44E3-A32F-30A12E0B11F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118CF0FD-675B-45F5-BD6E-8F58F391388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Geburtshilfe</t>
   </si>
   <si>
-    <t>Neonatologie</t>
-  </si>
-  <si>
-    <t>Kantonsspital Graubünden</t>
-  </si>
-  <si>
     <t>46.861556296686246</t>
   </si>
   <si>
@@ -68,18 +62,12 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>Spital Oberengadin</t>
-  </si>
-  <si>
     <t>46.5398337613234</t>
   </si>
   <si>
     <t>9.878987964240668</t>
   </si>
   <si>
-    <t>Regionalspital Surselva</t>
-  </si>
-  <si>
     <t>46.77706472897187</t>
   </si>
   <si>
@@ -104,27 +92,18 @@
     <t>9.686234727259531</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Spital Thusis</t>
   </si>
   <si>
     <t>Nein</t>
   </si>
   <si>
-    <t>Gesundheitszentrum Unterengadin</t>
-  </si>
-  <si>
     <t>46.7999988668582</t>
   </si>
   <si>
     <t>10.303826533438096</t>
   </si>
   <si>
-    <t>Ja?</t>
-  </si>
-  <si>
     <t>Centro sanitario Valposchiavo</t>
   </si>
   <si>
@@ -134,9 +113,6 @@
     <t>10.062210768116891</t>
   </si>
   <si>
-    <t>Ente Ospedaliero Cantonale (EOC)</t>
-  </si>
-  <si>
     <t>46.184275341809496</t>
   </si>
   <si>
@@ -174,6 +150,24 @@
   </si>
   <si>
     <t>SPITAL_Bellinzona</t>
+  </si>
+  <si>
+    <t>Kantonsspital Graubünden, Chur</t>
+  </si>
+  <si>
+    <t>Spital Oberengadin, Samedan</t>
+  </si>
+  <si>
+    <t>Regionalspital Surselva, Ilanz</t>
+  </si>
+  <si>
+    <t>Gesundheitszentrum Unterengadin, Scuol</t>
+  </si>
+  <si>
+    <t>Ente Ospedaliero Cantonale (EOC), Bellinzona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein </t>
   </si>
 </sst>
 </file>
@@ -562,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,7 +571,7 @@
     <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,210 +587,180 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">

</xml_diff>